<commit_message>
Knoppen hier, due dates daar, Joeri en zijn sloerie houden van mekaar
</commit_message>
<xml_diff>
--- a/data/job_data2.xlsx
+++ b/data/job_data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\python\OBP\OBP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD16B1CE-7FB2-4561-97A3-9764E1329A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9035CD-5AD5-4A4A-BC33-72EEFBC78F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3732" yWindow="576" windowWidth="17256" windowHeight="9384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -552,7 +552,7 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>5</v>

</xml_diff>

<commit_message>
Laatste touches Chefs' kiss
</commit_message>
<xml_diff>
--- a/data/job_data2.xlsx
+++ b/data/job_data2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\python\OBP\OBP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9035CD-5AD5-4A4A-BC33-72EEFBC78F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83706292-534D-4DAB-A58E-EA4E157CB839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="576" windowWidth="17256" windowHeight="9384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="732" windowWidth="17256" windowHeight="9384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,44 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>job_id</t>
-  </si>
-  <si>
-    <t>release_date</t>
-  </si>
-  <si>
-    <t>due_date</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>st_1</t>
-  </si>
-  <si>
-    <t>st_2</t>
-  </si>
-  <si>
-    <t>st_3</t>
-  </si>
-  <si>
-    <t>st_4</t>
-  </si>
-  <si>
-    <t>st_5</t>
-  </si>
-  <si>
-    <t>st_6</t>
-  </si>
-  <si>
-    <t>st_7</t>
-  </si>
-  <si>
-    <t>st_8</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,48 +385,24 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -539,44 +478,6 @@
       </c>
       <c r="L3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>9</v>
-      </c>
-      <c r="L4">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>